<commit_message>
Update atomic assertions parts of  PMA vplan
Signed-off-by: Kristine Dosvik <krdosvik@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/privileged_spec/CV32E40SX_PMA_VerifPlan.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/privileged_spec/CV32E40SX_PMA_VerifPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ropeders\Documents\pma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krdosvik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B73B54E-2C76-41DF-8A14-7A3F36FB8B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3614E6-7205-4E20-A66B-67137CF63CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-level Feature" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="240">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -164,9 +164,6 @@
  cause a precise store access fault (exception code 7).</t>
   </si>
   <si>
-    <t>Atomic operations</t>
-  </si>
-  <si>
     <t>Atomic operations shall only occur for regions in which Atomic operations are allowed. (Only applies for cores with A-extension)</t>
   </si>
   <si>
@@ -325,19 +322,10 @@
     <t>Region index or default IO unmapped region crossed with passing load instruction</t>
   </si>
   <si>
-    <t>Atomic instruction coverpoint</t>
-  </si>
-  <si>
     <t>Load alignment error coverpoint</t>
   </si>
   <si>
     <t>Store alignment error coverpoint</t>
-  </si>
-  <si>
-    <t>Atomic load-reserved unallowed error coverpoint</t>
-  </si>
-  <si>
-    <t>Atomic store-conditional unallowed error coverpoint</t>
   </si>
   <si>
     <t>Instruction fetch violation coverpoints</t>
@@ -411,14 +399,6 @@
   </si>
   <si>
     <t>Debug mode</t>
-  </si>
-  <si>
-    <t>PMA_NUM_REGIONS==0: 
-Accesses not matching attribute regions should be treated as: 
-Memory
-Non-Bufferable
-Non-Cacheable
-Atomic operations not allowed</t>
   </si>
   <si>
     <t>PMA_NUM_REGIONS&gt;0
@@ -427,14 +407,6 @@
 Non-Bufferable
 Non-Cacheable
 Atomic operations not allowed</t>
-  </si>
-  <si>
-    <t>Arbitrary accesses to non-configured PMA-areas.
-Self checking test should attempt the following: 
-- Non-aligned load/store accesses: should pass
-- Atomic lr/sc operations (if supported by core): should fail
-- Cacheable/Bufferable operations - verify instr and data_memtype[x] for correct behavior. (Assertions in OBI section should apply)
-- Instruction fetch and execute: should pass</t>
   </si>
   <si>
     <t>Arbitrary accesses to non-configured PMA-areas.
@@ -731,9 +703,6 @@
     <t>DTC: cv32e40s/tests/programs/custom/pma_debug/</t>
   </si>
   <si>
-    <t>(N/A for 40s)</t>
-  </si>
-  <si>
     <t>Assert that highest numbered PMA region &lt; 16 (assuming 0-indexed)
 Cover: Having 0 regions, having maximum num regions, and having something in between.</t>
   </si>
@@ -844,15 +813,7 @@
 COV: *pma_cov_*_i.cover_item_covergroup_cg_inst_cg_inst_coverpoint_cp_multimatch*</t>
   </si>
   <si>
-    <t>RTC: TODO
-COV: *pma_cov_*_i.cover_item_covergroup_cg_inst_cg_inst_cross_x_multimatch_aligned_loadstoreexec_*</t>
-  </si>
-  <si>
     <t>TODO is the random stream run without pma regions?</t>
-  </si>
-  <si>
-    <t>RTC: cv32e40s/tests/programs/corev-dv/corev_rand_pma_test/
-COV: *pma_cov_*_i.cover_item_covergroup_cg_inst_cg_inst_cross_x_multimatch_aligned_loadstoreexec_*</t>
   </si>
   <si>
     <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.core_i.if_stage_i.mpu_i.pma_assert_instr_i.a_req_prohibited
@@ -937,13 +898,66 @@
   </si>
   <si>
     <t xml:space="preserve"> -------END---------</t>
+  </si>
+  <si>
+    <t>40x: Atomic operations</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>PMA_NUM_REGIONS==0: 
+Accesses not matching attribute regions should be treated as: 
+Memory
+Non-Bufferable
+Non-Cacheable
+Atomic operations allowed</t>
+  </si>
+  <si>
+    <t>Arbitrary accesses to non-configured PMA-areas.
+Self checking test should attempt the following: 
+- Non-aligned load/store accesses: should pass
+- Atomic lr/sc operations (if supported by core): should pass
+- Cacheable/Bufferable operations - verify instr and data_memtype[x] for correct behavior. (Assertions in OBI section should apply)
+- Instruction fetch and execute: should pass</t>
+  </si>
+  <si>
+    <t>(40X) Atomic instruction coverpoint</t>
+  </si>
+  <si>
+    <t>(40X )Atomic load-reserved unallowed error coverpoint</t>
+  </si>
+  <si>
+    <t>(40X) Atomic store-conditional unallowed error coverpoint</t>
+  </si>
+  <si>
+    <t>COV: *x_lrw_firstfail*</t>
+  </si>
+  <si>
+    <t>COV: *x_scw_firstfail*</t>
+  </si>
+  <si>
+    <t>RTC: TODO
+A: TODO, a_atomic_access_no_pma_regions_LRW, a_atomic_access_no_pma_regions_SCW
+COV: *pma_cov_*_i.cover_item_covergroup_cg_inst_cg_inst_cross_x_multimatch_aligned_loadstoreexec_*</t>
+  </si>
+  <si>
+    <t>RTC: cv32e40s/tests/programs/corev-dv/corev_rand_pma_test/
+A: TODO, a_atomic_access_outside_pma_regions_LRW, a_atomic_access_outside_pma_regions_SCW
+COV: *pma_cov_*_i.cover_item_covergroup_cg_inst_cg_inst_cross_x_multimatch_aligned_loadstoreexec_*</t>
+  </si>
+  <si>
+    <t>A:  a_atomic_access_atomic_regions_LRW, a_atomic_access_nonatomic_regions_LRW</t>
+  </si>
+  <si>
+    <t>A: a_atomic_access_atomic_regions_SCW, a_atomic_access_nonatomic_regions_SCW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1051,7 +1065,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1088,16 +1102,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1487,28 +1504,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="B47" zoomScale="72" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.90625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.54296875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="24.08984375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="60.453125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="89.36328125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.36328125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="56.90625" style="12" customWidth="1"/>
-    <col min="10" max="10" width="23.36328125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="89.42578125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="56.85546875" style="12" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" style="12" customWidth="1"/>
     <col min="11" max="1023" width="17" style="12"/>
-    <col min="1024" max="1024" width="9.08984375" style="12" customWidth="1"/>
+    <col min="1024" max="1024" width="9.140625" style="12" customWidth="1"/>
     <col min="1025" max="16384" width="17" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="11" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="11" customFormat="1" ht="30">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1537,24 +1554,24 @@
         <v>8</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="315" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="315" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="D2" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>18</v>
@@ -1566,23 +1583,23 @@
         <v>14</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="154" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14" t="s">
-        <v>157</v>
+        <v>201</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="142.5">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16" t="s">
+        <v>151</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>21</v>
@@ -1596,19 +1613,19 @@
       <c r="I3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="126" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="J3" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="128.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="12" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>21</v>
@@ -1623,15 +1640,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+    <row r="5" spans="1:10" ht="42.75">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="12" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>21</v>
@@ -1646,15 +1663,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="112" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+    <row r="6" spans="1:10" ht="114">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="12" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>21</v>
@@ -1669,15 +1686,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="238" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+    <row r="7" spans="1:10" ht="242.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="12" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>21</v>
@@ -1692,15 +1709,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="238" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+    <row r="8" spans="1:10" ht="242.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="12" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>21</v>
@@ -1715,15 +1732,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="266" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+    <row r="9" spans="1:10" ht="270.75">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="12" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>21</v>
@@ -1738,17 +1755,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14" t="s">
+    <row r="10" spans="1:10" ht="180" customHeight="1">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>15</v>
@@ -1760,21 +1777,21 @@
         <v>14</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="56" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="57">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>15</v>
@@ -1786,18 +1803,18 @@
         <v>14</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="56" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="57">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>15</v>
@@ -1809,18 +1826,18 @@
         <v>14</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="12" t="s">
-        <v>94</v>
+        <v>231</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>23</v>
@@ -1832,15 +1849,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="56" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+    <row r="14" spans="1:10" ht="57">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>15</v>
@@ -1852,18 +1869,18 @@
         <v>14</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="56" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="57">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>15</v>
@@ -1875,64 +1892,70 @@
         <v>14</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="28.5">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="12" t="s">
-        <v>97</v>
+        <v>232</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="28.5">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="12" t="s">
-        <v>98</v>
+        <v>233</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="28" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="28.5">
       <c r="A18" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="D18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>49</v>
-      </c>
       <c r="E18" s="12" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>23</v>
@@ -1944,21 +1967,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="A19" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="14" t="s">
+    <row r="19" spans="1:10" ht="28.5">
+      <c r="A19" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="D19" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>104</v>
+      <c r="E19" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>9</v>
@@ -1970,15 +1993,15 @@
         <v>11</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="106.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="106.35" customHeight="1">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="12" t="s">
         <v>15</v>
       </c>
@@ -1989,20 +2012,20 @@
         <v>14</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="42" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="42.75">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>24</v>
@@ -2013,28 +2036,28 @@
       <c r="H21" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="126" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="14" t="s">
+      <c r="I21" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="128.25">
+      <c r="A22" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>126</v>
+      <c r="D22" s="16" t="s">
+        <v>120</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>18</v>
@@ -2046,16 +2069,16 @@
         <v>17</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="126" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14" t="s">
-        <v>55</v>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="128.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>18</v>
@@ -2067,15 +2090,15 @@
         <v>25</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="149" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="149.1" customHeight="1">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
       <c r="F24" s="12" t="s">
         <v>15</v>
       </c>
@@ -2086,20 +2109,20 @@
         <v>14</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>210</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="28.5">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>203</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>15</v>
@@ -2110,19 +2133,19 @@
       <c r="H25" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+      <c r="I25" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="96" customHeight="1">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
       <c r="F26" s="12" t="s">
         <v>15</v>
       </c>
@@ -2133,15 +2156,15 @@
         <v>14</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="124.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="124.35" customHeight="1">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="12" t="s">
         <v>18</v>
       </c>
@@ -2152,20 +2175,20 @@
         <v>17</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>124</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="28.5">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>9</v>
@@ -2177,15 +2200,15 @@
         <v>11</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="70" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="102" customHeight="1">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="12" t="s">
         <v>15</v>
       </c>
@@ -2195,22 +2218,22 @@
       <c r="H29" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="J29" s="16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>125</v>
+      <c r="I29" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="28.5">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>119</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>9</v>
@@ -2221,19 +2244,19 @@
       <c r="H30" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="92.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
+      <c r="I30" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="135" customHeight="1">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
       <c r="F31" s="12" t="s">
         <v>15</v>
       </c>
@@ -2243,25 +2266,25 @@
       <c r="H31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I31" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="238" x14ac:dyDescent="0.35">
-      <c r="A32" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="14" t="s">
+      <c r="I31" s="18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="242.25">
+      <c r="A32" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>67</v>
+      <c r="C32" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>18</v>
@@ -2273,14 +2296,14 @@
         <v>14</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="238" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="242.25">
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
       <c r="E33" s="12" t="s">
         <v>31</v>
       </c>
@@ -2294,15 +2317,15 @@
         <v>14</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="112" x14ac:dyDescent="0.35">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14" t="s">
-        <v>68</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="99.75">
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>32</v>
@@ -2317,14 +2340,14 @@
         <v>14</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="98" x14ac:dyDescent="0.35">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="99.75">
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
       <c r="E35" s="12" t="s">
         <v>33</v>
       </c>
@@ -2338,18 +2361,18 @@
         <v>14</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="112" x14ac:dyDescent="0.35">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="99.75">
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>18</v>
@@ -2361,20 +2384,20 @@
         <v>14</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="182" x14ac:dyDescent="0.35">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>66</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="185.25">
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>65</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>18</v>
@@ -2386,16 +2409,16 @@
         <v>14</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="182" x14ac:dyDescent="0.35">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="171">
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
       <c r="E38" s="12" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>18</v>
@@ -2407,14 +2430,14 @@
         <v>14</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="112" x14ac:dyDescent="0.35">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="114">
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16" t="s">
         <v>34</v>
       </c>
       <c r="E39" s="12" t="s">
@@ -2430,14 +2453,14 @@
         <v>14</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="112" x14ac:dyDescent="0.35">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="114">
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
       <c r="E40" s="12" t="s">
         <v>36</v>
       </c>
@@ -2451,18 +2474,18 @@
         <v>14</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="112" x14ac:dyDescent="0.35">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="114">
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>18</v>
@@ -2474,24 +2497,24 @@
         <v>14</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="54.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="14" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="54.6" customHeight="1">
+      <c r="A42" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="14" t="s">
-        <v>169</v>
+      <c r="E42" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="F42" s="12" t="s">
         <v>9</v>
@@ -2502,19 +2525,19 @@
       <c r="H42" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I42" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="J42" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="115.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
+      <c r="I42" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="115.35" customHeight="1">
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
       <c r="F43" s="12" t="s">
         <v>15</v>
       </c>
@@ -2524,22 +2547,22 @@
       <c r="H43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I43" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="J43" s="16" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14" t="s">
+      <c r="I43" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="33.6" customHeight="1">
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="14" t="s">
-        <v>170</v>
+      <c r="E44" s="16" t="s">
+        <v>164</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>9</v>
@@ -2551,15 +2574,15 @@
         <v>11</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="135" customHeight="1">
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
       <c r="F45" s="12" t="s">
         <v>15</v>
       </c>
@@ -2569,24 +2592,24 @@
       <c r="H45" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I45" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="J45" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>135</v>
+      <c r="I45" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="J45" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="41.1" customHeight="1">
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>9</v>
@@ -2597,19 +2620,19 @@
       <c r="H46" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="J46" s="16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="274.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
+      <c r="I46" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="274.5" customHeight="1">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
       <c r="F47" s="12" t="s">
         <v>18</v>
       </c>
@@ -2620,18 +2643,18 @@
         <v>14</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>134</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="48" customHeight="1">
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>9</v>
@@ -2643,15 +2666,15 @@
         <v>11</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="192" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="192" customHeight="1">
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
       <c r="F49" s="12" t="s">
         <v>15</v>
       </c>
@@ -2662,18 +2685,18 @@
         <v>14</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>136</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="47.25" customHeight="1">
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="F50" s="12" t="s">
         <v>9</v>
@@ -2684,19 +2707,19 @@
       <c r="H50" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I50" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="J50" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="200.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
+      <c r="I50" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J50" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="200.25" customHeight="1">
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
       <c r="F51" s="12" t="s">
         <v>15</v>
       </c>
@@ -2707,24 +2730,24 @@
         <v>14</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="35.1" customHeight="1">
+      <c r="A52" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>129</v>
+      <c r="E52" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="F52" s="12" t="s">
         <v>9</v>
@@ -2735,19 +2758,19 @@
       <c r="H52" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="J52" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="126.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
+      <c r="I52" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J52" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="126.6" customHeight="1">
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
       <c r="F53" s="12" t="s">
         <v>15</v>
       </c>
@@ -2757,24 +2780,24 @@
       <c r="H53" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I53" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="J53" s="16" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="40.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>128</v>
+      <c r="I53" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="J53" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="40.35" customHeight="1">
+      <c r="A54" s="16"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="F54" s="12" t="s">
         <v>9</v>
@@ -2785,19 +2808,19 @@
       <c r="H54" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I54" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="J54" s="16" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="127.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
+      <c r="I54" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="127.35" customHeight="1">
+      <c r="A55" s="16"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
       <c r="F55" s="12" t="s">
         <v>15</v>
       </c>
@@ -2807,24 +2830,24 @@
       <c r="H55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I55" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="J55" s="16" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="104" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>139</v>
+      <c r="I55" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="J55" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="104.1" customHeight="1">
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>9</v>
@@ -2835,20 +2858,20 @@
       <c r="H56" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I56" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="J56" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="49.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
+      <c r="I56" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J56" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="49.35" customHeight="1">
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
       <c r="E57" s="12" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>9</v>
@@ -2859,20 +2882,20 @@
       <c r="H57" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I57" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="J57" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="199.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
+      <c r="I57" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J57" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="199.35" customHeight="1">
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
       <c r="E58" s="12" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>15</v>
@@ -2883,24 +2906,24 @@
       <c r="H58" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I58" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="J58" s="16" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="56" x14ac:dyDescent="0.35">
+      <c r="I58" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="J58" s="14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="57">
       <c r="A59" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
+        <v>132</v>
+      </c>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
       <c r="D59" s="12" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>9</v>
@@ -2911,28 +2934,28 @@
       <c r="H59" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I59" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="56" x14ac:dyDescent="0.35">
-      <c r="A60" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>121</v>
+      <c r="I59" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="J59" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="57">
+      <c r="A60" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F60" s="12" t="s">
         <v>9</v>
@@ -2944,20 +2967,20 @@
         <v>11</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="42" x14ac:dyDescent="0.35">
-      <c r="A61" s="14"/>
-      <c r="B61" s="14"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="42.75">
+      <c r="A61" s="16"/>
+      <c r="B61" s="16"/>
       <c r="C61" s="12" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>9</v>
@@ -2969,24 +2992,24 @@
         <v>11</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="195.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="195.6" customHeight="1">
       <c r="A62" s="12" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>18</v>
@@ -2998,24 +3021,24 @@
         <v>20</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="A63" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B63" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="28.5">
+      <c r="A63" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C63" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="D63" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D63" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>102</v>
+      <c r="E63" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>9</v>
@@ -3027,15 +3050,15 @@
         <v>11</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="69" customHeight="1">
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
       <c r="F64" s="12" t="s">
         <v>15</v>
       </c>
@@ -3046,18 +3069,18 @@
         <v>14</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>103</v>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="28.5">
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="F65" s="12" t="s">
         <v>9</v>
@@ -3069,15 +3092,15 @@
         <v>11</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="63.75" customHeight="1">
+      <c r="A66" s="16"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
       <c r="F66" s="12" t="s">
         <v>15</v>
       </c>
@@ -3088,24 +3111,24 @@
         <v>14</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="85.5">
       <c r="A67" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F67" s="12" t="s">
         <v>15</v>
@@ -3116,28 +3139,28 @@
       <c r="H67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I67" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="J67" s="16" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="198.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I67" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="J67" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="198.6" customHeight="1">
       <c r="A68" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F68" s="12" t="s">
         <v>18</v>
@@ -3149,21 +3172,21 @@
         <v>14</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="B73" s="15"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="15"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="15"/>
-      <c r="H73" s="15"/>
-      <c r="I73" s="15"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="13" customFormat="1">
+      <c r="A73" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="64">
@@ -3244,7 +3267,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>H2:H22 H90:H103 H24:H88</xm:sqref>
+          <xm:sqref>H24:H88 H90:H103 H2:H22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -3284,17 +3307,17 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" style="1"/>
-    <col min="3" max="3" width="32.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" style="1"/>
-    <col min="5" max="5" width="23.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.6328125" style="1"/>
+    <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="1"/>
+    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="1"/>
+    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -3307,7 +3330,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3318,7 +3341,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3329,7 +3352,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -3340,7 +3363,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -3351,7 +3374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -3362,7 +3385,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -3370,7 +3393,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -3378,7 +3401,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
@@ -3397,17 +3420,17 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.90625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="72.54296875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="130.90625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="53.453125" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="11.54296875" style="6"/>
+    <col min="1" max="1" width="2.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="72.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="130.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="11.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="15">
       <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
@@ -3421,60 +3444,60 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5">
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5">
       <c r="B4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="6" t="s">
+    </row>
+    <row r="5" spans="2:5" ht="42.75">
+      <c r="B5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="42" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="2:5" ht="15">
       <c r="B6" s="6" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15">
       <c r="B7" s="6" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3501,54 +3524,54 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.6328125" customWidth="1"/>
-    <col min="2" max="2" width="77.54296875" customWidth="1"/>
-    <col min="3" max="3" width="74.6328125" customWidth="1"/>
-    <col min="4" max="4" width="62.08984375" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="77.5703125" customWidth="1"/>
+    <col min="3" max="3" width="74.5703125" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="120.95" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="120.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="84.6" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="84.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove TODO with description of why link to coverage does not exit
Signed-off-by: Kristine Dosvik <krdosvik@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/privileged_spec/CV32E40SX_PMA_VerifPlan.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/privileged_spec/CV32E40SX_PMA_VerifPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krdosvik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3614E6-7205-4E20-A66B-67137CF63CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890CF93D-D13C-4E0B-A3EE-21FADEB62D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-level Feature" sheetId="1" r:id="rId1"/>
@@ -903,9 +903,6 @@
     <t>40x: Atomic operations</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>PMA_NUM_REGIONS==0: 
 Accesses not matching attribute regions should be treated as: 
 Memory
@@ -951,6 +948,9 @@
   </si>
   <si>
     <t>A: a_atomic_access_atomic_regions_SCW, a_atomic_access_nonatomic_regions_SCW</t>
+  </si>
+  <si>
+    <t>Fow now: covered by assertions only.</t>
   </si>
 </sst>
 </file>
@@ -1108,13 +1108,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1504,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" zoomScale="72" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="72" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="14.25"/>
@@ -1558,10 +1558,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="315" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="12" t="s">
@@ -1590,9 +1590,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="142.5">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D3" s="12" t="s">
@@ -1618,9 +1618,9 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="128.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="12" t="s">
         <v>158</v>
       </c>
@@ -1641,9 +1641,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="42.75">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="12" t="s">
         <v>157</v>
       </c>
@@ -1664,9 +1664,9 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="114">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="12" t="s">
         <v>154</v>
       </c>
@@ -1687,9 +1687,9 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="242.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="12" t="s">
         <v>155</v>
       </c>
@@ -1710,9 +1710,9 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="242.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="12" t="s">
         <v>156</v>
       </c>
@@ -1733,9 +1733,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="270.75">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="12" t="s">
         <v>166</v>
       </c>
@@ -1756,9 +1756,9 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="180" customHeight="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17" t="s">
         <v>84</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -1784,9 +1784,9 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="57">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="12" t="s">
         <v>82</v>
       </c>
@@ -1807,9 +1807,9 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="57">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="12" t="s">
         <v>83</v>
       </c>
@@ -1830,11 +1830,11 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>87</v>
@@ -1850,9 +1850,9 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="57">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="12" t="s">
         <v>93</v>
       </c>
@@ -1873,9 +1873,9 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="57">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="12" t="s">
         <v>94</v>
       </c>
@@ -1896,11 +1896,11 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.5">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>91</v>
@@ -1915,15 +1915,15 @@
         <v>14</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="28.5">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>90</v>
@@ -1938,7 +1938,7 @@
         <v>14</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="28.5">
@@ -1968,19 +1968,19 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="28.5">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="17" t="s">
         <v>100</v>
       </c>
       <c r="F19" s="12" t="s">
@@ -1997,11 +1997,11 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="106.35" customHeight="1">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="12" t="s">
         <v>15</v>
       </c>
@@ -2016,8 +2016,8 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="42.75">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="12" t="s">
         <v>95</v>
       </c>
@@ -2044,16 +2044,16 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="128.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="17" t="s">
         <v>120</v>
       </c>
       <c r="E22" s="12" t="s">
@@ -2073,11 +2073,11 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="128.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17" t="s">
         <v>54</v>
       </c>
       <c r="F23" s="12" t="s">
@@ -2094,11 +2094,11 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="149.1" customHeight="1">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="12" t="s">
         <v>15</v>
       </c>
@@ -2113,15 +2113,15 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="28.5">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16" t="s">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="17" t="s">
         <v>203</v>
       </c>
       <c r="F25" s="12" t="s">
@@ -2141,11 +2141,11 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="96" customHeight="1">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="12" t="s">
         <v>15</v>
       </c>
@@ -2160,11 +2160,11 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="124.35" customHeight="1">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="12" t="s">
         <v>18</v>
       </c>
@@ -2179,16 +2179,16 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="28.5">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16" t="s">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="E28" s="17" t="s">
         <v>229</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>230</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>9</v>
@@ -2204,11 +2204,11 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="102" customHeight="1">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="12" t="s">
         <v>15</v>
       </c>
@@ -2219,20 +2219,20 @@
         <v>14</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J29" s="14" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="28.5">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16" t="s">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="17" t="s">
         <v>119</v>
       </c>
       <c r="F30" s="12" t="s">
@@ -2252,11 +2252,11 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="135" customHeight="1">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="12" t="s">
         <v>15</v>
       </c>
@@ -2266,21 +2266,21 @@
       <c r="H31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I31" s="18" t="s">
-        <v>237</v>
+      <c r="I31" s="16" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="242.25">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="17" t="s">
         <v>66</v>
       </c>
       <c r="E32" s="12" t="s">
@@ -2300,10 +2300,10 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="242.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
       <c r="E33" s="12" t="s">
         <v>31</v>
       </c>
@@ -2321,10 +2321,10 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="99.75">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16" t="s">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17" t="s">
         <v>67</v>
       </c>
       <c r="E34" s="12" t="s">
@@ -2344,10 +2344,10 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="99.75">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
       <c r="E35" s="12" t="s">
         <v>33</v>
       </c>
@@ -2365,9 +2365,9 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="99.75">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="12" t="s">
         <v>101</v>
       </c>
@@ -2388,12 +2388,12 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="185.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16" t="s">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="17" t="s">
         <v>65</v>
       </c>
       <c r="E37" s="12" t="s">
@@ -2413,10 +2413,10 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="171">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
       <c r="E38" s="12" t="s">
         <v>191</v>
       </c>
@@ -2434,10 +2434,10 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="114">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16" t="s">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E39" s="12" t="s">
@@ -2457,10 +2457,10 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="114">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
       <c r="E40" s="12" t="s">
         <v>36</v>
       </c>
@@ -2478,9 +2478,9 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="114">
-      <c r="A41" s="16"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
       <c r="D41" s="12" t="s">
         <v>102</v>
       </c>
@@ -2501,19 +2501,19 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="54.6" customHeight="1">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E42" s="17" t="s">
         <v>163</v>
       </c>
       <c r="F42" s="12" t="s">
@@ -2533,11 +2533,11 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="115.35" customHeight="1">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
       <c r="F43" s="12" t="s">
         <v>15</v>
       </c>
@@ -2555,13 +2555,13 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="33.6" customHeight="1">
-      <c r="A44" s="16"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16" t="s">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="17" t="s">
         <v>164</v>
       </c>
       <c r="F44" s="12" t="s">
@@ -2578,11 +2578,11 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="135" customHeight="1">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
       <c r="F45" s="12" t="s">
         <v>15</v>
       </c>
@@ -2600,15 +2600,15 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="41.1" customHeight="1">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16" t="s">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E46" s="17" t="s">
         <v>129</v>
       </c>
       <c r="F46" s="12" t="s">
@@ -2628,11 +2628,11 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="274.5" customHeight="1">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
       <c r="F47" s="12" t="s">
         <v>18</v>
       </c>
@@ -2647,13 +2647,13 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="48" customHeight="1">
-      <c r="A48" s="16"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16" t="s">
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="E48" s="17" t="s">
         <v>128</v>
       </c>
       <c r="F48" s="12" t="s">
@@ -2670,11 +2670,11 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="192" customHeight="1">
-      <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
       <c r="F49" s="12" t="s">
         <v>15</v>
       </c>
@@ -2689,13 +2689,13 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="47.25" customHeight="1">
-      <c r="A50" s="16"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16" t="s">
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="E50" s="16" t="s">
+      <c r="E50" s="17" t="s">
         <v>130</v>
       </c>
       <c r="F50" s="12" t="s">
@@ -2715,11 +2715,11 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="200.25" customHeight="1">
-      <c r="A51" s="16"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
       <c r="F51" s="12" t="s">
         <v>15</v>
       </c>
@@ -2734,19 +2734,19 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="35.1" customHeight="1">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="17" t="s">
         <v>123</v>
       </c>
       <c r="F52" s="12" t="s">
@@ -2766,11 +2766,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="126.6" customHeight="1">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
       <c r="F53" s="12" t="s">
         <v>15</v>
       </c>
@@ -2788,15 +2788,15 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="40.35" customHeight="1">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16" t="s">
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="E54" s="17" t="s">
         <v>122</v>
       </c>
       <c r="F54" s="12" t="s">
@@ -2816,11 +2816,11 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="127.35" customHeight="1">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
+      <c r="A55" s="17"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
       <c r="F55" s="12" t="s">
         <v>15</v>
       </c>
@@ -2838,12 +2838,12 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="104.1" customHeight="1">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16" t="s">
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="17" t="s">
         <v>133</v>
       </c>
       <c r="E56" s="12" t="s">
@@ -2866,10 +2866,10 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="49.35" customHeight="1">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
       <c r="E57" s="12" t="s">
         <v>134</v>
       </c>
@@ -2890,10 +2890,10 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="199.35" customHeight="1">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
       <c r="E58" s="12" t="s">
         <v>137</v>
       </c>
@@ -2917,8 +2917,8 @@
       <c r="A59" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
       <c r="D59" s="12" t="s">
         <v>131</v>
       </c>
@@ -2942,10 +2942,10 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="57">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="17" t="s">
         <v>117</v>
       </c>
       <c r="C60" s="12" t="s">
@@ -2971,8 +2971,8 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="42.75">
-      <c r="A61" s="16"/>
-      <c r="B61" s="16"/>
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="12" t="s">
         <v>138</v>
       </c>
@@ -3025,19 +3025,19 @@
       </c>
     </row>
     <row r="63" spans="1:10" ht="28.5">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="17" t="s">
         <v>98</v>
       </c>
       <c r="F63" s="12" t="s">
@@ -3050,15 +3050,15 @@
         <v>11</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="69" customHeight="1">
-      <c r="A64" s="16"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
       <c r="F64" s="12" t="s">
         <v>15</v>
       </c>
@@ -3069,17 +3069,17 @@
         <v>14</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="28.5">
-      <c r="A65" s="16"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16" t="s">
+      <c r="A65" s="17"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="E65" s="17" t="s">
         <v>99</v>
       </c>
       <c r="F65" s="12" t="s">
@@ -3092,15 +3092,15 @@
         <v>11</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A66" s="16"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
       <c r="F66" s="12" t="s">
         <v>15</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>14</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="85.5">
@@ -3176,32 +3176,56 @@
       </c>
     </row>
     <row r="73" spans="1:10" s="13" customFormat="1">
-      <c r="A73" s="17" t="s">
+      <c r="A73" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="17"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B52:B59"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B17"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C3:C9"/>
+    <mergeCell ref="B32:B41"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="A73:I73"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E63:E64"/>
     <mergeCell ref="A22:A31"/>
     <mergeCell ref="B22:B31"/>
     <mergeCell ref="C28:C31"/>
@@ -3218,42 +3242,18 @@
     <mergeCell ref="D48:D49"/>
     <mergeCell ref="D46:D47"/>
     <mergeCell ref="A32:A41"/>
-    <mergeCell ref="B32:B41"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="A73:I73"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B17"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C3:C9"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B52:B59"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C54:C55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>